<commit_message>
Added background image and removed link to update.php in the navbar
</commit_message>
<xml_diff>
--- a/mktime webstore project/Improvements_to_MKPedals.xlsx
+++ b/mktime webstore project/Improvements_to_MKPedals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\EC Web Technologies\mktime webstore project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAD225F-FB45-4795-B258-86FBB1A2698B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC62454-3C14-4656-A39B-9517B9DCDDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14565" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{487F07B6-2726-4F52-8D2A-6FF46137F293}"/>
+    <workbookView xWindow="4910" yWindow="0" windowWidth="14400" windowHeight="8170" xr2:uid="{487F07B6-2726-4F52-8D2A-6FF46137F293}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Page</t>
   </si>
@@ -149,6 +149,27 @@
   </si>
   <si>
     <t>Found a CRUD example page that included exactly this. Also deleted the PHP code in the value attribute of each field in the form because it wasn't needed since I put a header in underneath to redirect to the view page.</t>
+  </si>
+  <si>
+    <t>Add functionality to check if email address is already in database</t>
+  </si>
+  <si>
+    <t>Look at the Moodle and Sharon's example code if possible</t>
+  </si>
+  <si>
+    <t>Adjust padding and transparency of cards</t>
+  </si>
+  <si>
+    <t>create.php</t>
+  </si>
+  <si>
+    <t>Add div containing the form so it's visible against the background image</t>
+  </si>
+  <si>
+    <t>Tidy up form fields</t>
+  </si>
+  <si>
+    <t>Stop them from being full-width</t>
   </si>
 </sst>
 </file>
@@ -621,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911854F4-99CB-4E35-BCFD-3721A9321F35}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E12" activeCellId="1" sqref="C15 E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,34 +813,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D12" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="D15" s="3" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Fixed top padding and create page redirect
</commit_message>
<xml_diff>
--- a/mktime webstore project/Improvements_to_MKPedals.xlsx
+++ b/mktime webstore project/Improvements_to_MKPedals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\EC Web Technologies\mktime webstore project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC62454-3C14-4656-A39B-9517B9DCDDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7751102-64F8-43B1-9676-7F7DE0FC1080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4910" yWindow="0" windowWidth="14400" windowHeight="8170" xr2:uid="{487F07B6-2726-4F52-8D2A-6FF46137F293}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" xr2:uid="{487F07B6-2726-4F52-8D2A-6FF46137F293}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Page</t>
   </si>
@@ -170,6 +170,24 @@
   </si>
   <si>
     <t>Stop them from being full-width</t>
+  </si>
+  <si>
+    <t>Add functionality to show "In stock"/"Out of stock"</t>
+  </si>
+  <si>
+    <t>nav.php</t>
+  </si>
+  <si>
+    <t>Ensure it highlights the name of the current page in the navbar</t>
+  </si>
+  <si>
+    <t>Bootstrap has built-in functionality for this (the "active" class) so it took some PHP to insert a conditional statement that looks at the page name using the $_SERVER superglobal and inserts "active" into the class attribute if it matches.</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Get the background to work</t>
   </si>
 </sst>
 </file>
@@ -642,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911854F4-99CB-4E35-BCFD-3721A9321F35}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E12" activeCellId="1" sqref="C15 E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -865,31 +883,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -897,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -905,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -913,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -921,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -929,7 +962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -937,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -945,7 +978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -953,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -961,7 +994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -969,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -977,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -985,7 +1018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -993,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>

</xml_diff>

<commit_message>
Implemented login and logout functionality as well as pages which can only be viewed when logged in
</commit_message>
<xml_diff>
--- a/mktime webstore project/Improvements_to_MKPedals.xlsx
+++ b/mktime webstore project/Improvements_to_MKPedals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\EC Web Technologies\mktime webstore project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7751102-64F8-43B1-9676-7F7DE0FC1080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BADB50-7B2D-4C18-87CC-B52A0691199F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" xr2:uid="{487F07B6-2726-4F52-8D2A-6FF46137F293}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{487F07B6-2726-4F52-8D2A-6FF46137F293}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Page</t>
   </si>
@@ -188,6 +188,18 @@
   </si>
   <si>
     <t>Get the background to work</t>
+  </si>
+  <si>
+    <t>Scroll animations?</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=0TnO1GzKWPc&amp;ab_channel=SnippetsCode</t>
+  </si>
+  <si>
+    <t>Ensure you can only sign up with an email address once</t>
+  </si>
+  <si>
+    <t>You'll probably need to add a clause that checks the database for that email address (if ($row &gt; 0) { return "This email address is already registered."}</t>
   </si>
 </sst>
 </file>
@@ -660,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911854F4-99CB-4E35-BCFD-3721A9321F35}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -923,17 +935,29 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="D19" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+    <row r="20" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="D20" s="3" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Created admin login functionality
</commit_message>
<xml_diff>
--- a/mktime webstore project/Improvements_to_MKPedals.xlsx
+++ b/mktime webstore project/Improvements_to_MKPedals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\EC Web Technologies\mktime webstore project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BADB50-7B2D-4C18-87CC-B52A0691199F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DD5D25-DB2A-4453-9773-753DA890010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{487F07B6-2726-4F52-8D2A-6FF46137F293}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="52">
   <si>
     <t>Page</t>
   </si>
@@ -201,12 +201,27 @@
   <si>
     <t>You'll probably need to add a clause that checks the database for that email address (if ($row &gt; 0) { return "This email address is already registered."}</t>
   </si>
+  <si>
+    <t>Create admin login functionality</t>
+  </si>
+  <si>
+    <t>Added to login_tools and login_action, creating an 'admin' key for the $_SESSION global</t>
+  </si>
+  <si>
+    <t>Create shopping cart functionality</t>
+  </si>
+  <si>
+    <t>Cre</t>
+  </si>
+  <si>
+    <t>Also add the option to add payment methods and add fields for this to the database</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +245,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -248,10 +271,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -267,8 +291,12 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -672,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911854F4-99CB-4E35-BCFD-3721A9321F35}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -842,6 +870,9 @@
       <c r="D11" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
@@ -854,7 +885,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -934,14 +965,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="3" t="b">
@@ -959,28 +990,42 @@
         <v>46</v>
       </c>
       <c r="D20" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="D21" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="3" t="b">
         <v>0</v>
@@ -1203,9 +1248,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C19" r:id="rId1" xr:uid="{FD6D948A-E14A-4C72-8FD6-45AFDB36685D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed background image, added item filter view, adjusted spacing and transparency of cards, and ensured admin-only access to certain pages
</commit_message>
<xml_diff>
--- a/mktime webstore project/Improvements_to_MKPedals.xlsx
+++ b/mktime webstore project/Improvements_to_MKPedals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\EC Web Technologies\mktime webstore project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DD5D25-DB2A-4453-9773-753DA890010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC7A796-5DDA-428D-B2CB-BBFFFEAD2109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{487F07B6-2726-4F52-8D2A-6FF46137F293}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Page</t>
   </si>
@@ -211,10 +211,16 @@
     <t>Create shopping cart functionality</t>
   </si>
   <si>
-    <t>Cre</t>
-  </si>
-  <si>
     <t>Also add the option to add payment methods and add fields for this to the database</t>
+  </si>
+  <si>
+    <t>read.php/admin_read.php</t>
+  </si>
+  <si>
+    <t>Improve the filter dropdown to dynamically update when new effects types are added</t>
+  </si>
+  <si>
+    <t>Could probably take all of the effects types under "effect_type" in the database, push them to an array and use a loop to echo them all to the dropdown list</t>
   </si>
 </sst>
 </file>
@@ -368,8 +374,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F3AFA12B-219D-450B-B05A-BEE248E7BA34}" name="Table2" displayName="Table2" ref="A1:E50" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E50" xr:uid="{F3AFA12B-219D-450B-B05A-BEE248E7BA34}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F3AFA12B-219D-450B-B05A-BEE248E7BA34}" name="Table2" displayName="Table2" ref="A1:E49" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E49" xr:uid="{F3AFA12B-219D-450B-B05A-BEE248E7BA34}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B94D3DFC-872B-4478-BBC8-E28D92ADEE28}" name="Page" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{11523FCA-8CE9-4067-9AF0-7CE4808C59D4}" name="Improvement" dataDxfId="3"/>
@@ -698,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911854F4-99CB-4E35-BCFD-3721A9321F35}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -767,7 +773,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -779,7 +785,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -871,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -897,7 +903,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -909,7 +915,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -923,7 +929,7 @@
         <v>36</v>
       </c>
       <c r="D15" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -962,7 +968,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -1019,14 +1025,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="D23" s="3" t="b">
         <v>0</v>
       </c>
@@ -1236,14 +1244,6 @@
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="3" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added shopping cart and checkout functionality
</commit_message>
<xml_diff>
--- a/mktime webstore project/Improvements_to_MKPedals.xlsx
+++ b/mktime webstore project/Improvements_to_MKPedals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\EC Web Technologies\mktime webstore project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A08ADD5-F58F-4F4E-9D29-DCACE24724A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE17746C-E1AD-449B-B67E-4F71CF69398B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" xr2:uid="{487F07B6-2726-4F52-8D2A-6FF46137F293}"/>
+    <workbookView xWindow="-14565" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{487F07B6-2726-4F52-8D2A-6FF46137F293}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Page</t>
   </si>
@@ -224,6 +224,12 @@
   </si>
   <si>
     <t>Make it log you out when the session is disconnected</t>
+  </si>
+  <si>
+    <t>Sort out files into folders</t>
+  </si>
+  <si>
+    <t>Will require editing all the hrefs within all the files</t>
   </si>
 </sst>
 </file>
@@ -709,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911854F4-99CB-4E35-BCFD-3721A9321F35}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1054,10 +1060,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D25" s="3" t="b">
         <v>0</v>
       </c>

</xml_diff>